<commit_message>
Added rows in KeywordDriven
</commit_message>
<xml_diff>
--- a/KeywordDriven/src/main/resources/TestSuite.xlsx
+++ b/KeywordDriven/src/main/resources/TestSuite.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGitLabRepos\Java-Automation-Frameworks\KeywordDriven\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGitLabRepos\Java-Automation-Frameworks\KeywordDriven\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Sr.No.</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>Anything Relevant</t>
+  </si>
+  <si>
+    <t>amazon</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>TEST-002</t>
   </si>
 </sst>
 </file>
@@ -449,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -485,7 +494,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -502,7 +513,9 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -515,16 +528,71 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>